<commit_message>
Update on 20220929 (Maybe the last commit on LiuLin@ChinaTelecom)
</commit_message>
<xml_diff>
--- a/文档/其他文档/年度小结文档/2022年度每月工作总结/公式/需求统计数据汇总.xlsx
+++ b/文档/其他文档/年度小结文档/2022年度每月工作总结/公式/需求统计数据汇总.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" activeTab="7"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2022.1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="36">
   <si>
     <t>总共</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -165,6 +165,14 @@
   </si>
   <si>
     <t>截止统计版本：2022-09-06终稿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>截止统计版本：2022-10-11终稿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>综合资源管理系统(IRM)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3710,6 +3718,418 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <f>61+74+44+93+53</f>
+        <v>325</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <f>24+26+16+24+26</f>
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <f>6+10+3+5+5</f>
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <f>18+15+12+19+21</f>
+        <v>85</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <f>8+5+5+1</f>
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <f>5+4+4+1</f>
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3">
+        <f>2+1+1</f>
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <f>32+32+20+50+20</f>
+        <v>154</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <f>17+11+6+22+7</f>
+        <v>63</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2">
+        <f>15+19+14+27+13</f>
+        <v>88</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2">
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <f>4+5+3+13+6</f>
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <f>2+1+2+2+2</f>
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <f>2+4+1+10+3</f>
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3">
+        <f>1+2+1</f>
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3">
+        <f>1+2+1</f>
+        <v>4</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <f>SUM(D2:D10)</f>
+        <v>115</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM(F2:F10)</f>
+        <v>202</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4">
+        <f>SUM(H2:H10)</f>
+        <v>7</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="4">
+        <f>SUM(J2:J10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3725,8 +4145,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <f>61+74+44+93+53</f>
-        <v>325</v>
+        <f>64+50+81+36</f>
+        <v>231</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3742,36 +4162,36 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>24+26+16+24+26</f>
-        <v>116</v>
+        <f>20+21+25</f>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <f>6+10+3+5+5</f>
+        <f>1+19+9</f>
         <v>29</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1">
-        <f>18+15+12+19+21</f>
-        <v>85</v>
+        <f>18+2+10</f>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <f>1+1</f>
-        <v>2</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="1">
-        <f>0</f>
-        <v>0</v>
+        <f>1+6</f>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
@@ -3779,22 +4199,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <f>8+5+5+1</f>
-        <v>19</v>
+        <f>3+4+3</f>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3">
-        <f>5+4+4+1</f>
-        <v>14</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <f>2+1+1</f>
-        <v>4</v>
+        <f>3+3+3</f>
+        <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
@@ -3807,8 +4227,8 @@
         <v>13</v>
       </c>
       <c r="J3" s="3">
-        <f>1</f>
-        <v>1</v>
+        <f>0</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
@@ -3816,29 +4236,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <f>32+32+20+50+20</f>
-        <v>154</v>
+        <f>34+18+47+31</f>
+        <v>130</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2">
-        <f>17+11+6+22+7</f>
-        <v>63</v>
+        <f>17+9+19+12</f>
+        <v>57</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <f>15+19+14+27+13</f>
-        <v>88</v>
+        <f>17+9+27+19</f>
+        <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2">
-        <f>2+1</f>
-        <v>3</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
@@ -3853,15 +4273,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f>1+1</f>
+        <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="8">
-        <f>0</f>
-        <v>0</v>
+        <f>1+1</f>
+        <v>2</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>9</v>
@@ -3890,29 +4310,29 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <f>4+5+3+13+6</f>
-        <v>31</v>
+        <f>6+7+7+2</f>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3">
-        <f>2+1+2+2+2</f>
-        <v>9</v>
+        <f>5+3+2+2</f>
+        <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <f>2+4+1+10+3</f>
-        <v>20</v>
+        <f>1+4+5</f>
+        <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="3">
-        <f>1+1</f>
-        <v>2</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>13</v>
@@ -3964,8 +4384,8 @@
         <v>32</v>
       </c>
       <c r="B8" s="3">
-        <f>1+2+1</f>
-        <v>4</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -3978,8 +4398,8 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <f>1+2+1</f>
-        <v>4</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>11</v>
@@ -4080,289 +4500,34 @@
       </c>
       <c r="D11" s="4">
         <f>SUM(D2:D10)</f>
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(F2:F10)</f>
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="4">
         <f>SUM(H2:H10)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="4">
         <f>SUM(J2:J10)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="G13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="8"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="4"/>
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update on 20221231 (Goodbye 2022)
</commit_message>
<xml_diff>
--- a/文档/其他文档/年度小结文档/2022年度每月工作总结/公式/需求统计数据汇总.xlsx
+++ b/文档/其他文档/年度小结文档/2022年度每月工作总结/公式/需求统计数据汇总.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="165" windowWidth="19395" windowHeight="7575" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="2022.1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>截止统计版本：2023-1-3终稿</t>
+    <t>截止统计版本：2023-1-3终稿
+（统计截至2022.12.29,2023年不再统计！）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -304,7 +305,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -340,6 +341,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1433,6 +1437,416 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <f>38+83+61+57+45</f>
+        <v>284</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <f>5+32+23+22+14</f>
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <f>3+7+7+13+1</f>
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <f>24+15+9+13</f>
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
+        <f>2+1+1</f>
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <f>7+3+3+5+2</f>
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3">
+        <f>7+2+3+3+2</f>
+        <v>17</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <f>25+45+26+27+25</f>
+        <v>148</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <f>10+20+9+16+9</f>
+        <v>64</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="2">
+        <f>15+25+17+10+15</f>
+        <v>82</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <f>1+2+5+3+4</f>
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <f>1+2+2+2+1</f>
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3">
+        <f>2+3+1</f>
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="3">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="5">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <f>SUM(D2:D10)</f>
+        <v>107</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM(F2:F10)</f>
+        <v>170</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="4">
+        <f>SUM(H2:H10)</f>
+        <v>7</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="4">
+        <f>SUM(J2:J10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1448,8 +1862,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <f>38+83+61+57+45</f>
-        <v>284</v>
+        <f>39+42+80+40</f>
+        <v>201</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1465,29 +1879,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>5+32+23+22+14</f>
-        <v>96</v>
+        <f>9+14+10+2</f>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <f>3+7+7+13+1</f>
-        <v>31</v>
+        <f>1+5+2+1</f>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="1">
-        <f>24+15+9+13</f>
-        <v>61</v>
+        <f>8+9+8+1</f>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <f>2+1+1</f>
-        <v>4</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -1502,22 +1916,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <f>7+3+3+5+2</f>
-        <v>20</v>
+        <f>6+2+4</f>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="3">
-        <f>1+2</f>
-        <v>3</v>
+        <f>1+4</f>
+        <v>5</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="3">
-        <f>7+2+3+3+2</f>
-        <v>17</v>
+        <f>5+2</f>
+        <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
@@ -1539,29 +1953,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <f>25+45+26+27+25</f>
-        <v>148</v>
+        <f>22+25+57+38</f>
+        <v>142</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2">
-        <f>10+20+9+16+9</f>
-        <v>64</v>
+        <f>11+15+34+14</f>
+        <v>74</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="2">
-        <f>15+25+17+10+15</f>
-        <v>82</v>
+        <f>10+10+22+23</f>
+        <v>65</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="2">
-        <f>1</f>
-        <v>1</v>
+        <f>1+1+1</f>
+        <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
@@ -1613,29 +2027,29 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <f>1+2+5+3+4</f>
-        <v>15</v>
+        <f>2+1+8</f>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="3">
-        <f>1+2+2+2+1</f>
-        <v>8</v>
+        <f>2+4</f>
+        <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <f>2+3+1</f>
-        <v>6</v>
+        <f>1+3</f>
+        <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="3">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>13</v>
@@ -1650,8 +2064,8 @@
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <f>2</f>
-        <v>2</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -1664,8 +2078,8 @@
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <f>2</f>
-        <v>2</v>
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>11</v>
@@ -1687,8 +2101,8 @@
         <v>32</v>
       </c>
       <c r="B8" s="3">
-        <f>1+1</f>
-        <v>2</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -1701,8 +2115,8 @@
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <f>1+1</f>
-        <v>2</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>11</v>
@@ -1724,15 +2138,15 @@
         <v>14</v>
       </c>
       <c r="B9" s="6">
-        <f>1</f>
-        <v>1</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="6">
-        <f>1</f>
-        <v>1</v>
+        <f>0</f>
+        <v>0</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>9</v>
@@ -1803,21 +2217,21 @@
       </c>
       <c r="D11" s="4">
         <f>SUM(D2:D10)</f>
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(F2:F10)</f>
-        <v>170</v>
+        <v>103</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="4">
         <f>SUM(H2:H10)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>13</v>
@@ -1827,415 +2241,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="G13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="8">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="6">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="6">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="6">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="5">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="5">
-        <f>0</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4">
-        <f>SUM(D2:D10)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="4">
-        <f>SUM(F2:F10)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="4">
-        <f>SUM(H2:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="4">
-        <f>SUM(J2:J10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="G13" t="s">
+    <row r="13" spans="1:10" ht="27" x14ac:dyDescent="0.15">
+      <c r="G13" s="12" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>